<commit_message>
Mejoras programa pruebas y stats completos
</commit_message>
<xml_diff>
--- a/Codigo/Codigo-GEM5/salida.xlsx
+++ b/Codigo/Codigo-GEM5/salida.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15512" uniqueCount="11060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15512" uniqueCount="11051">
   <si>
     <t xml:space="preserve">simFreq</t>
   </si>
@@ -31351,25 +31351,10 @@
     <t xml:space="preserve">3053.98</t>
   </si>
   <si>
-    <t xml:space="preserve">0.010017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.010062</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.010254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.781286</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.034488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.034644</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.035305</t>
+    <t xml:space="preserve">0.743460</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.005578</t>
   </si>
   <si>
     <t xml:space="preserve">776826402</t>
@@ -31927,22 +31912,10 @@
     <t xml:space="preserve">3102.94</t>
   </si>
   <si>
-    <t xml:space="preserve">0.010022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.010058</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.010081</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.034511</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.034636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.034713</t>
+    <t xml:space="preserve">0.743467</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000273</t>
   </si>
   <si>
     <t xml:space="preserve">776719761</t>
@@ -33289,13 +33262,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -33317,14 +33294,17 @@
   </sheetPr>
   <dimension ref="A1:IT1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="II49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="IZ67" activeCellId="0" sqref="IZ67"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P65" activeCellId="0" sqref="P65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="23.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="12.57"/>
@@ -77604,7 +77584,7 @@
         <v>10436</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>254</v>
       </c>
@@ -77629,179 +77609,179 @@
       <c r="H63" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="I63" s="0" t="s">
-        <v>10441</v>
+      <c r="I63" s="2" t="s">
+        <v>10443</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>10443</v>
+        <v>4817</v>
       </c>
       <c r="K63" s="0" t="s">
+        <v>934</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="N63" s="0" t="s">
+        <v>5571</v>
+      </c>
+      <c r="O63" s="0" t="s">
         <v>10444</v>
       </c>
-      <c r="L63" s="0" t="s">
+      <c r="P63" s="0" t="s">
+        <v>5385</v>
+      </c>
+      <c r="Q63" s="0" t="s">
         <v>10445</v>
       </c>
-      <c r="M63" s="0" t="s">
+      <c r="R63" s="0" t="s">
         <v>10446</v>
       </c>
-      <c r="N63" s="0" t="s">
+      <c r="S63" s="0" t="s">
         <v>10447</v>
       </c>
-      <c r="O63" s="0" t="s">
+      <c r="T63" s="0" t="s">
         <v>10448</v>
       </c>
-      <c r="P63" s="0" t="s">
+      <c r="U63" s="0" t="s">
         <v>10449</v>
       </c>
-      <c r="Q63" s="0" t="s">
+      <c r="V63" s="0" t="s">
         <v>10450</v>
       </c>
-      <c r="R63" s="0" t="s">
+      <c r="W63" s="0" t="s">
         <v>10451</v>
       </c>
-      <c r="S63" s="0" t="s">
+      <c r="X63" s="0" t="s">
         <v>10452</v>
       </c>
-      <c r="T63" s="0" t="s">
+      <c r="Y63" s="0" t="s">
         <v>10453</v>
       </c>
-      <c r="U63" s="0" t="s">
+      <c r="Z63" s="0" t="s">
         <v>10454</v>
       </c>
-      <c r="V63" s="0" t="s">
+      <c r="AA63" s="0" t="s">
         <v>10455</v>
       </c>
-      <c r="W63" s="0" t="s">
+      <c r="AB63" s="0" t="s">
         <v>10456</v>
       </c>
-      <c r="X63" s="0" t="s">
+      <c r="AC63" s="0" t="s">
         <v>10457</v>
       </c>
-      <c r="Y63" s="0" t="s">
+      <c r="AD63" s="0" t="s">
         <v>10458</v>
       </c>
-      <c r="Z63" s="0" t="s">
+      <c r="AE63" s="0" t="s">
         <v>10459</v>
       </c>
-      <c r="AA63" s="0" t="s">
+      <c r="AF63" s="0" t="s">
         <v>10460</v>
       </c>
-      <c r="AB63" s="0" t="s">
+      <c r="AG63" s="0" t="s">
+        <v>10457</v>
+      </c>
+      <c r="AH63" s="0" t="s">
         <v>10461</v>
       </c>
-      <c r="AC63" s="0" t="s">
+      <c r="AI63" s="0" t="s">
+        <v>10458</v>
+      </c>
+      <c r="AJ63" s="0" t="s">
         <v>10462</v>
       </c>
-      <c r="AD63" s="0" t="s">
+      <c r="AK63" s="0" t="s">
+        <v>10459</v>
+      </c>
+      <c r="AL63" s="0" t="s">
         <v>10463</v>
       </c>
-      <c r="AE63" s="0" t="s">
+      <c r="AM63" s="0" t="s">
+        <v>10460</v>
+      </c>
+      <c r="AN63" s="0" t="s">
         <v>10464</v>
       </c>
-      <c r="AF63" s="0" t="s">
+      <c r="AO63" s="0" t="s">
         <v>10465</v>
       </c>
-      <c r="AG63" s="0" t="s">
-        <v>10462</v>
-      </c>
-      <c r="AH63" s="0" t="s">
+      <c r="AP63" s="0" t="s">
         <v>10466</v>
       </c>
-      <c r="AI63" s="0" t="s">
-        <v>10463</v>
-      </c>
-      <c r="AJ63" s="0" t="s">
+      <c r="AQ63" s="0" t="s">
         <v>10467</v>
       </c>
-      <c r="AK63" s="0" t="s">
-        <v>10464</v>
-      </c>
-      <c r="AL63" s="0" t="s">
+      <c r="AR63" s="0" t="s">
         <v>10468</v>
       </c>
-      <c r="AM63" s="0" t="s">
-        <v>10465</v>
-      </c>
-      <c r="AN63" s="0" t="s">
+      <c r="AS63" s="0" t="s">
         <v>10469</v>
       </c>
-      <c r="AO63" s="0" t="s">
+      <c r="AT63" s="0" t="s">
         <v>10470</v>
       </c>
-      <c r="AP63" s="0" t="s">
+      <c r="AU63" s="0" t="s">
         <v>10471</v>
       </c>
-      <c r="AQ63" s="0" t="s">
+      <c r="AV63" s="0" t="s">
         <v>10472</v>
       </c>
-      <c r="AR63" s="0" t="s">
+      <c r="AW63" s="0" t="s">
         <v>10473</v>
       </c>
-      <c r="AS63" s="0" t="s">
+      <c r="AX63" s="0" t="s">
         <v>10474</v>
       </c>
-      <c r="AT63" s="0" t="s">
+      <c r="AY63" s="0" t="s">
         <v>10475</v>
       </c>
-      <c r="AU63" s="0" t="s">
+      <c r="AZ63" s="0" t="s">
         <v>10476</v>
       </c>
-      <c r="AV63" s="0" t="s">
+      <c r="BA63" s="0" t="s">
         <v>10477</v>
       </c>
-      <c r="AW63" s="0" t="s">
+      <c r="BB63" s="0" t="s">
         <v>10478</v>
       </c>
-      <c r="AX63" s="0" t="s">
+      <c r="BC63" s="0" t="s">
         <v>10479</v>
       </c>
-      <c r="AY63" s="0" t="s">
+      <c r="BD63" s="0" t="s">
         <v>10480</v>
       </c>
-      <c r="AZ63" s="0" t="s">
+      <c r="BE63" s="0" t="s">
         <v>10481</v>
       </c>
-      <c r="BA63" s="0" t="s">
+      <c r="BF63" s="0" t="s">
         <v>10482</v>
       </c>
-      <c r="BB63" s="0" t="s">
+      <c r="BG63" s="0" t="s">
         <v>10483</v>
       </c>
-      <c r="BC63" s="0" t="s">
+      <c r="BH63" s="0" t="s">
         <v>10484</v>
       </c>
-      <c r="BD63" s="0" t="s">
+      <c r="BI63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="BJ63" s="0" t="s">
         <v>10485</v>
       </c>
-      <c r="BE63" s="0" t="s">
+      <c r="BK63" s="0" t="s">
         <v>10486</v>
       </c>
-      <c r="BF63" s="0" t="s">
+      <c r="BL63" s="0" t="s">
         <v>10487</v>
       </c>
-      <c r="BG63" s="0" t="s">
+      <c r="BM63" s="0" t="s">
         <v>10488</v>
       </c>
-      <c r="BH63" s="0" t="s">
+      <c r="BN63" s="0" t="s">
         <v>10489</v>
-      </c>
-      <c r="BI63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="BJ63" s="0" t="s">
-        <v>10490</v>
-      </c>
-      <c r="BK63" s="0" t="s">
-        <v>10491</v>
-      </c>
-      <c r="BL63" s="0" t="s">
-        <v>10492</v>
-      </c>
-      <c r="BM63" s="0" t="s">
-        <v>10493</v>
-      </c>
-      <c r="BN63" s="0" t="s">
-        <v>10494</v>
       </c>
       <c r="BO63" s="0" t="s">
         <v>310</v>
@@ -77813,166 +77793,166 @@
         <v>310</v>
       </c>
       <c r="BR63" s="0" t="s">
+        <v>10490</v>
+      </c>
+      <c r="BS63" s="0" t="s">
+        <v>10491</v>
+      </c>
+      <c r="BT63" s="0" t="s">
+        <v>10492</v>
+      </c>
+      <c r="BU63" s="0" t="s">
+        <v>10493</v>
+      </c>
+      <c r="BV63" s="0" t="s">
+        <v>10494</v>
+      </c>
+      <c r="BW63" s="0" t="s">
         <v>10495</v>
       </c>
-      <c r="BS63" s="0" t="s">
+      <c r="BX63" s="0" t="s">
         <v>10496</v>
       </c>
-      <c r="BT63" s="0" t="s">
+      <c r="BY63" s="0" t="s">
         <v>10497</v>
       </c>
-      <c r="BU63" s="0" t="s">
+      <c r="BZ63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CA63" s="0" t="s">
         <v>10498</v>
       </c>
-      <c r="BV63" s="0" t="s">
+      <c r="CB63" s="0" t="s">
         <v>10499</v>
       </c>
-      <c r="BW63" s="0" t="s">
+      <c r="CC63" s="0" t="s">
         <v>10500</v>
       </c>
-      <c r="BX63" s="0" t="s">
+      <c r="CD63" s="0" t="s">
         <v>10501</v>
       </c>
-      <c r="BY63" s="0" t="s">
+      <c r="CE63" s="0" t="s">
         <v>10502</v>
       </c>
-      <c r="BZ63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CA63" s="0" t="s">
+      <c r="CF63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CG63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CH63" s="0" t="s">
         <v>10503</v>
       </c>
-      <c r="CB63" s="0" t="s">
+      <c r="CI63" s="0" t="s">
         <v>10504</v>
       </c>
-      <c r="CC63" s="0" t="s">
+      <c r="CJ63" s="0" t="s">
         <v>10505</v>
       </c>
-      <c r="CD63" s="0" t="s">
+      <c r="CK63" s="0" t="s">
         <v>10506</v>
       </c>
-      <c r="CE63" s="0" t="s">
+      <c r="CL63" s="0" t="s">
         <v>10507</v>
       </c>
-      <c r="CF63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CG63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CH63" s="0" t="s">
+      <c r="CM63" s="0" t="s">
         <v>10508</v>
       </c>
-      <c r="CI63" s="0" t="s">
+      <c r="CN63" s="0" t="s">
         <v>10509</v>
       </c>
-      <c r="CJ63" s="0" t="s">
+      <c r="CO63" s="0" t="s">
         <v>10510</v>
       </c>
-      <c r="CK63" s="0" t="s">
+      <c r="CP63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CQ63" s="0" t="s">
         <v>10511</v>
       </c>
-      <c r="CL63" s="0" t="s">
+      <c r="CR63" s="0" t="s">
         <v>10512</v>
       </c>
-      <c r="CM63" s="0" t="s">
+      <c r="CS63" s="0" t="s">
         <v>10513</v>
       </c>
-      <c r="CN63" s="0" t="s">
+      <c r="CT63" s="0" t="s">
         <v>10514</v>
       </c>
-      <c r="CO63" s="0" t="s">
+      <c r="CU63" s="0" t="s">
         <v>10515</v>
       </c>
-      <c r="CP63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CQ63" s="0" t="s">
+      <c r="CV63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CW63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CX63" s="0" t="s">
         <v>10516</v>
       </c>
-      <c r="CR63" s="0" t="s">
+      <c r="CY63" s="0" t="s">
         <v>10517</v>
       </c>
-      <c r="CS63" s="0" t="s">
+      <c r="CZ63" s="0" t="s">
         <v>10518</v>
       </c>
-      <c r="CT63" s="0" t="s">
+      <c r="DA63" s="0" t="s">
         <v>10519</v>
       </c>
-      <c r="CU63" s="0" t="s">
+      <c r="DB63" s="0" t="s">
         <v>10520</v>
       </c>
-      <c r="CV63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CW63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CX63" s="0" t="s">
+      <c r="DC63" s="0" t="s">
         <v>10521</v>
       </c>
-      <c r="CY63" s="0" t="s">
+      <c r="DD63" s="0" t="s">
         <v>10522</v>
       </c>
-      <c r="CZ63" s="0" t="s">
+      <c r="DE63" s="0" t="s">
         <v>10523</v>
       </c>
-      <c r="DA63" s="0" t="s">
+      <c r="DF63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG63" s="0" t="s">
         <v>10524</v>
       </c>
-      <c r="DB63" s="0" t="s">
+      <c r="DH63" s="0" t="s">
         <v>10525</v>
       </c>
-      <c r="DC63" s="0" t="s">
+      <c r="DI63" s="0" t="s">
         <v>10526</v>
       </c>
-      <c r="DD63" s="0" t="s">
+      <c r="DJ63" s="0" t="s">
         <v>10527</v>
       </c>
-      <c r="DE63" s="0" t="s">
+      <c r="DK63" s="0" t="s">
         <v>10528</v>
       </c>
-      <c r="DF63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG63" s="0" t="s">
+      <c r="DL63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DN63" s="0" t="s">
         <v>10529</v>
       </c>
-      <c r="DH63" s="0" t="s">
+      <c r="DO63" s="0" t="s">
         <v>10530</v>
       </c>
-      <c r="DI63" s="0" t="s">
+      <c r="DP63" s="0" t="s">
         <v>10531</v>
       </c>
-      <c r="DJ63" s="0" t="s">
+      <c r="DQ63" s="0" t="s">
         <v>10532</v>
       </c>
-      <c r="DK63" s="0" t="s">
+      <c r="DR63" s="0" t="s">
         <v>10533</v>
       </c>
-      <c r="DL63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DN63" s="0" t="s">
+      <c r="DS63" s="0" t="s">
         <v>10534</v>
-      </c>
-      <c r="DO63" s="0" t="s">
-        <v>10535</v>
-      </c>
-      <c r="DP63" s="0" t="s">
-        <v>10536</v>
-      </c>
-      <c r="DQ63" s="0" t="s">
-        <v>10537</v>
-      </c>
-      <c r="DR63" s="0" t="s">
-        <v>10538</v>
-      </c>
-      <c r="DS63" s="0" t="s">
-        <v>10539</v>
       </c>
       <c r="DT63" s="0" t="s">
         <v>6276</v>
@@ -77981,22 +77961,22 @@
         <v>365</v>
       </c>
       <c r="DV63" s="0" t="s">
-        <v>10540</v>
+        <v>10535</v>
       </c>
       <c r="DW63" s="0" t="s">
-        <v>10541</v>
+        <v>10536</v>
       </c>
       <c r="DX63" s="0" t="s">
         <v>366</v>
       </c>
       <c r="DY63" s="0" t="s">
-        <v>10542</v>
+        <v>10537</v>
       </c>
       <c r="DZ63" s="0" t="s">
-        <v>10543</v>
+        <v>10538</v>
       </c>
       <c r="EA63" s="0" t="s">
-        <v>10544</v>
+        <v>10539</v>
       </c>
       <c r="EB63" s="0" t="s">
         <v>310</v>
@@ -78005,58 +77985,58 @@
         <v>370</v>
       </c>
       <c r="ED63" s="0" t="s">
+        <v>10537</v>
+      </c>
+      <c r="EE63" s="0" t="s">
+        <v>10540</v>
+      </c>
+      <c r="EF63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="EG63" s="0" t="s">
+        <v>10541</v>
+      </c>
+      <c r="EH63" s="0" t="s">
         <v>10542</v>
       </c>
-      <c r="EE63" s="0" t="s">
+      <c r="EI63" s="0" t="s">
+        <v>10543</v>
+      </c>
+      <c r="EJ63" s="0" t="s">
+        <v>10544</v>
+      </c>
+      <c r="EK63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="EL63" s="0" t="s">
         <v>10545</v>
       </c>
-      <c r="EF63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="EG63" s="0" t="s">
+      <c r="EM63" s="0" t="s">
         <v>10546</v>
       </c>
-      <c r="EH63" s="0" t="s">
+      <c r="EN63" s="0" t="s">
         <v>10547</v>
-      </c>
-      <c r="EI63" s="0" t="s">
-        <v>10548</v>
-      </c>
-      <c r="EJ63" s="0" t="s">
-        <v>10549</v>
-      </c>
-      <c r="EK63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="EL63" s="0" t="s">
-        <v>10550</v>
-      </c>
-      <c r="EM63" s="0" t="s">
-        <v>10551</v>
-      </c>
-      <c r="EN63" s="0" t="s">
-        <v>10552</v>
       </c>
       <c r="EP63" s="0" t="s">
         <v>707</v>
       </c>
       <c r="EQ63" s="0" t="s">
-        <v>10553</v>
+        <v>10548</v>
       </c>
       <c r="ES63" s="0" t="s">
-        <v>10554</v>
+        <v>10549</v>
       </c>
       <c r="ET63" s="0" t="s">
         <v>366</v>
       </c>
       <c r="EV63" s="0" t="s">
-        <v>10555</v>
+        <v>10550</v>
       </c>
       <c r="EW63" s="0" t="s">
-        <v>10556</v>
+        <v>10551</v>
       </c>
       <c r="EX63" s="0" t="s">
-        <v>10557</v>
+        <v>10552</v>
       </c>
       <c r="EY63" s="0" t="s">
         <v>310</v>
@@ -78065,52 +78045,52 @@
         <v>370</v>
       </c>
       <c r="FA63" s="0" t="s">
+        <v>10550</v>
+      </c>
+      <c r="FB63" s="0" t="s">
+        <v>10553</v>
+      </c>
+      <c r="FC63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="FD63" s="0" t="s">
+        <v>10554</v>
+      </c>
+      <c r="FE63" s="0" t="s">
         <v>10555</v>
-      </c>
-      <c r="FB63" s="0" t="s">
-        <v>10558</v>
-      </c>
-      <c r="FC63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="FD63" s="0" t="s">
-        <v>10559</v>
-      </c>
-      <c r="FE63" s="0" t="s">
-        <v>10560</v>
       </c>
       <c r="FF63" s="0" t="s">
         <v>4738</v>
       </c>
       <c r="FG63" s="0" t="s">
-        <v>10561</v>
+        <v>10556</v>
       </c>
       <c r="FH63" s="0" t="s">
         <v>310</v>
       </c>
       <c r="FI63" s="0" t="s">
-        <v>10562</v>
+        <v>10557</v>
       </c>
       <c r="FJ63" s="0" t="s">
-        <v>10563</v>
+        <v>10558</v>
       </c>
       <c r="FK63" s="0" t="s">
-        <v>10564</v>
+        <v>10559</v>
       </c>
       <c r="FL63" s="0" t="s">
         <v>467</v>
       </c>
       <c r="FM63" s="0" t="s">
-        <v>10565</v>
+        <v>10560</v>
       </c>
       <c r="FN63" s="0" t="s">
-        <v>10566</v>
+        <v>10561</v>
       </c>
       <c r="FO63" s="0" t="s">
         <v>8441</v>
       </c>
       <c r="FP63" s="0" t="s">
-        <v>10567</v>
+        <v>10562</v>
       </c>
       <c r="FQ63" s="0" t="s">
         <v>722</v>
@@ -78119,13 +78099,13 @@
         <v>366</v>
       </c>
       <c r="FS63" s="0" t="s">
-        <v>10568</v>
+        <v>10563</v>
       </c>
       <c r="FT63" s="0" t="s">
-        <v>10569</v>
+        <v>10564</v>
       </c>
       <c r="FU63" s="0" t="s">
-        <v>10570</v>
+        <v>10565</v>
       </c>
       <c r="FV63" s="0" t="s">
         <v>310</v>
@@ -78134,67 +78114,67 @@
         <v>370</v>
       </c>
       <c r="FX63" s="0" t="s">
+        <v>10563</v>
+      </c>
+      <c r="FY63" s="0" t="s">
+        <v>10566</v>
+      </c>
+      <c r="FZ63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GA63" s="0" t="s">
+        <v>10567</v>
+      </c>
+      <c r="GB63" s="0" t="s">
         <v>10568</v>
-      </c>
-      <c r="FY63" s="0" t="s">
-        <v>10571</v>
-      </c>
-      <c r="FZ63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GA63" s="0" t="s">
-        <v>10572</v>
-      </c>
-      <c r="GB63" s="0" t="s">
-        <v>10573</v>
       </c>
       <c r="GC63" s="0" t="s">
         <v>3795</v>
       </c>
       <c r="GD63" s="0" t="s">
+        <v>10569</v>
+      </c>
+      <c r="GE63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GF63" s="0" t="s">
+        <v>10570</v>
+      </c>
+      <c r="GG63" s="0" t="s">
+        <v>10571</v>
+      </c>
+      <c r="GH63" s="0" t="s">
+        <v>10572</v>
+      </c>
+      <c r="GI63" s="0" t="s">
+        <v>10573</v>
+      </c>
+      <c r="GJ63" s="0" t="s">
         <v>10574</v>
       </c>
-      <c r="GE63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GF63" s="0" t="s">
+      <c r="GL63" s="0" t="s">
         <v>10575</v>
       </c>
-      <c r="GG63" s="0" t="s">
+      <c r="GM63" s="0" t="s">
         <v>10576</v>
       </c>
-      <c r="GH63" s="0" t="s">
+      <c r="GN63" s="0" t="s">
         <v>10577</v>
       </c>
-      <c r="GI63" s="0" t="s">
+      <c r="GO63" s="0" t="s">
         <v>10578</v>
-      </c>
-      <c r="GJ63" s="0" t="s">
-        <v>10579</v>
-      </c>
-      <c r="GL63" s="0" t="s">
-        <v>10580</v>
-      </c>
-      <c r="GM63" s="0" t="s">
-        <v>10581</v>
-      </c>
-      <c r="GN63" s="0" t="s">
-        <v>10582</v>
-      </c>
-      <c r="GO63" s="0" t="s">
-        <v>10583</v>
       </c>
       <c r="GP63" s="0" t="s">
         <v>2266</v>
       </c>
       <c r="GQ63" s="0" t="s">
-        <v>10584</v>
+        <v>10579</v>
       </c>
       <c r="GR63" s="0" t="s">
-        <v>10585</v>
+        <v>10580</v>
       </c>
       <c r="GS63" s="0" t="s">
-        <v>10586</v>
+        <v>10581</v>
       </c>
       <c r="GT63" s="0" t="s">
         <v>310</v>
@@ -78203,348 +78183,348 @@
         <v>370</v>
       </c>
       <c r="GV63" s="0" t="s">
+        <v>10579</v>
+      </c>
+      <c r="GW63" s="0" t="s">
+        <v>10582</v>
+      </c>
+      <c r="GX63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GY63" s="0" t="s">
+        <v>10583</v>
+      </c>
+      <c r="GZ63" s="0" t="s">
         <v>10584</v>
       </c>
-      <c r="GW63" s="0" t="s">
+      <c r="HA63" s="0" t="s">
+        <v>10585</v>
+      </c>
+      <c r="HB63" s="0" t="s">
+        <v>10586</v>
+      </c>
+      <c r="HC63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="HD63" s="0" t="s">
         <v>10587</v>
       </c>
-      <c r="GX63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GY63" s="0" t="s">
+      <c r="HE63" s="0" t="s">
         <v>10588</v>
       </c>
-      <c r="GZ63" s="0" t="s">
+      <c r="HF63" s="0" t="s">
         <v>10589</v>
       </c>
-      <c r="HA63" s="0" t="s">
+      <c r="HG63" s="0" t="s">
         <v>10590</v>
       </c>
-      <c r="HB63" s="0" t="s">
+      <c r="HH63" s="0" t="s">
         <v>10591</v>
       </c>
-      <c r="HC63" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="HD63" s="0" t="s">
+      <c r="HI63" s="0" t="s">
         <v>10592</v>
       </c>
-      <c r="HE63" s="0" t="s">
+      <c r="HJ63" s="0" t="s">
         <v>10593</v>
       </c>
-      <c r="HF63" s="0" t="s">
+      <c r="HK63" s="0" t="s">
         <v>10594</v>
       </c>
-      <c r="HG63" s="0" t="s">
+      <c r="HL63" s="0" t="s">
         <v>10595</v>
       </c>
-      <c r="HH63" s="0" t="s">
+      <c r="HM63" s="0" t="s">
         <v>10596</v>
       </c>
-      <c r="HI63" s="0" t="s">
+      <c r="HN63" s="0" t="s">
         <v>10597</v>
       </c>
-      <c r="HJ63" s="0" t="s">
+      <c r="HO63" s="0" t="s">
         <v>10598</v>
       </c>
-      <c r="HK63" s="0" t="s">
+      <c r="HP63" s="0" t="s">
         <v>10599</v>
       </c>
-      <c r="HL63" s="0" t="s">
+      <c r="HQ63" s="0" t="s">
         <v>10600</v>
       </c>
-      <c r="HM63" s="0" t="s">
+      <c r="HR63" s="0" t="s">
         <v>10601</v>
-      </c>
-      <c r="HN63" s="0" t="s">
-        <v>10602</v>
-      </c>
-      <c r="HO63" s="0" t="s">
-        <v>10603</v>
-      </c>
-      <c r="HP63" s="0" t="s">
-        <v>10604</v>
-      </c>
-      <c r="HQ63" s="0" t="s">
-        <v>10605</v>
-      </c>
-      <c r="HR63" s="0" t="s">
-        <v>10606</v>
       </c>
       <c r="HS63" s="0" t="s">
         <v>2119</v>
       </c>
       <c r="HT63" s="0" t="s">
-        <v>10607</v>
+        <v>10602</v>
       </c>
       <c r="HU63" s="0" t="s">
         <v>4400</v>
       </c>
       <c r="HV63" s="0" t="s">
+        <v>10603</v>
+      </c>
+      <c r="HW63" s="0" t="s">
+        <v>10604</v>
+      </c>
+      <c r="HX63" s="0" t="s">
+        <v>10605</v>
+      </c>
+      <c r="HY63" s="0" t="s">
+        <v>10606</v>
+      </c>
+      <c r="HZ63" s="0" t="s">
+        <v>10607</v>
+      </c>
+      <c r="IA63" s="0" t="s">
         <v>10608</v>
-      </c>
-      <c r="HW63" s="0" t="s">
-        <v>10609</v>
-      </c>
-      <c r="HX63" s="0" t="s">
-        <v>10610</v>
-      </c>
-      <c r="HY63" s="0" t="s">
-        <v>10611</v>
-      </c>
-      <c r="HZ63" s="0" t="s">
-        <v>10612</v>
-      </c>
-      <c r="IA63" s="0" t="s">
-        <v>10613</v>
       </c>
       <c r="IB63" s="0" t="s">
         <v>1052</v>
       </c>
       <c r="IC63" s="0" t="s">
+        <v>10609</v>
+      </c>
+      <c r="ID63" s="0" t="s">
+        <v>10610</v>
+      </c>
+      <c r="IE63" s="0" t="s">
+        <v>10611</v>
+      </c>
+      <c r="IF63" s="0" t="s">
+        <v>10612</v>
+      </c>
+      <c r="IG63" s="0" t="s">
+        <v>10613</v>
+      </c>
+      <c r="IH63" s="0" t="s">
         <v>10614</v>
       </c>
-      <c r="ID63" s="0" t="s">
+      <c r="II63" s="0" t="s">
         <v>10615</v>
       </c>
-      <c r="IE63" s="0" t="s">
+      <c r="IJ63" s="0" t="s">
         <v>10616</v>
       </c>
-      <c r="IF63" s="0" t="s">
+      <c r="IK63" s="0" t="s">
         <v>10617</v>
       </c>
-      <c r="IG63" s="0" t="s">
+      <c r="IL63" s="0" t="s">
         <v>10618</v>
       </c>
-      <c r="IH63" s="0" t="s">
+      <c r="IM63" s="0" t="s">
         <v>10619</v>
       </c>
-      <c r="II63" s="0" t="s">
+      <c r="IN63" s="0" t="s">
         <v>10620</v>
       </c>
-      <c r="IJ63" s="0" t="s">
+      <c r="IO63" s="0" t="s">
         <v>10621</v>
       </c>
-      <c r="IK63" s="0" t="s">
+      <c r="IP63" s="0" t="s">
         <v>10622</v>
       </c>
-      <c r="IL63" s="0" t="s">
+      <c r="IQ63" s="0" t="s">
         <v>10623</v>
       </c>
-      <c r="IM63" s="0" t="s">
-        <v>10624</v>
-      </c>
-      <c r="IN63" s="0" t="s">
-        <v>10625</v>
-      </c>
-      <c r="IO63" s="0" t="s">
-        <v>10626</v>
-      </c>
-      <c r="IP63" s="0" t="s">
-        <v>10627</v>
-      </c>
-      <c r="IQ63" s="0" t="s">
-        <v>10628</v>
-      </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>254</v>
       </c>
       <c r="B64" s="0" t="s">
+        <v>10624</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>10625</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>10626</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>10627</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>10628</v>
+      </c>
+      <c r="G64" s="0" t="s">
         <v>10629</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>10630</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>10631</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>10632</v>
-      </c>
-      <c r="F64" s="0" t="s">
-        <v>10633</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>10634</v>
       </c>
       <c r="H64" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="I64" s="0" t="s">
+      <c r="I64" s="2" t="s">
+        <v>10630</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>1965</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>10631</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="N64" s="0" t="s">
+        <v>2159</v>
+      </c>
+      <c r="O64" s="0" t="s">
+        <v>3665</v>
+      </c>
+      <c r="P64" s="0" t="s">
+        <v>6327</v>
+      </c>
+      <c r="Q64" s="0" t="s">
+        <v>10632</v>
+      </c>
+      <c r="R64" s="0" t="s">
         <v>10633</v>
       </c>
-      <c r="J64" s="0" t="s">
+      <c r="S64" s="0" t="s">
+        <v>10634</v>
+      </c>
+      <c r="T64" s="0" t="s">
         <v>10635</v>
       </c>
-      <c r="K64" s="0" t="s">
+      <c r="U64" s="0" t="s">
         <v>10636</v>
-      </c>
-      <c r="L64" s="0" t="s">
-        <v>10637</v>
-      </c>
-      <c r="M64" s="0" t="s">
-        <v>10446</v>
-      </c>
-      <c r="N64" s="0" t="s">
-        <v>10638</v>
-      </c>
-      <c r="O64" s="0" t="s">
-        <v>10639</v>
-      </c>
-      <c r="P64" s="0" t="s">
-        <v>10640</v>
-      </c>
-      <c r="Q64" s="0" t="s">
-        <v>10641</v>
-      </c>
-      <c r="R64" s="0" t="s">
-        <v>10642</v>
-      </c>
-      <c r="S64" s="0" t="s">
-        <v>10643</v>
-      </c>
-      <c r="T64" s="0" t="s">
-        <v>10644</v>
-      </c>
-      <c r="U64" s="0" t="s">
-        <v>10645</v>
       </c>
       <c r="V64" s="0" t="s">
         <v>4250</v>
       </c>
       <c r="W64" s="0" t="s">
-        <v>10646</v>
+        <v>10637</v>
       </c>
       <c r="X64" s="0" t="s">
-        <v>10647</v>
+        <v>10638</v>
       </c>
       <c r="Y64" s="0" t="s">
-        <v>10648</v>
+        <v>10639</v>
       </c>
       <c r="Z64" s="0" t="s">
         <v>4254</v>
       </c>
       <c r="AA64" s="0" t="s">
+        <v>10640</v>
+      </c>
+      <c r="AB64" s="0" t="s">
+        <v>10641</v>
+      </c>
+      <c r="AC64" s="0" t="s">
+        <v>10642</v>
+      </c>
+      <c r="AD64" s="0" t="s">
+        <v>10643</v>
+      </c>
+      <c r="AE64" s="0" t="s">
+        <v>10644</v>
+      </c>
+      <c r="AF64" s="0" t="s">
+        <v>10645</v>
+      </c>
+      <c r="AG64" s="0" t="s">
+        <v>10642</v>
+      </c>
+      <c r="AH64" s="0" t="s">
+        <v>10646</v>
+      </c>
+      <c r="AI64" s="0" t="s">
+        <v>10643</v>
+      </c>
+      <c r="AJ64" s="0" t="s">
+        <v>10647</v>
+      </c>
+      <c r="AK64" s="0" t="s">
+        <v>10644</v>
+      </c>
+      <c r="AL64" s="0" t="s">
+        <v>10648</v>
+      </c>
+      <c r="AM64" s="0" t="s">
+        <v>10645</v>
+      </c>
+      <c r="AN64" s="0" t="s">
         <v>10649</v>
       </c>
-      <c r="AB64" s="0" t="s">
+      <c r="AO64" s="0" t="s">
         <v>10650</v>
       </c>
-      <c r="AC64" s="0" t="s">
+      <c r="AP64" s="0" t="s">
         <v>10651</v>
       </c>
-      <c r="AD64" s="0" t="s">
+      <c r="AQ64" s="0" t="s">
         <v>10652</v>
       </c>
-      <c r="AE64" s="0" t="s">
+      <c r="AR64" s="0" t="s">
         <v>10653</v>
       </c>
-      <c r="AF64" s="0" t="s">
+      <c r="AS64" s="0" t="s">
         <v>10654</v>
       </c>
-      <c r="AG64" s="0" t="s">
-        <v>10651</v>
-      </c>
-      <c r="AH64" s="0" t="s">
+      <c r="AT64" s="0" t="s">
         <v>10655</v>
       </c>
-      <c r="AI64" s="0" t="s">
-        <v>10652</v>
-      </c>
-      <c r="AJ64" s="0" t="s">
+      <c r="AU64" s="0" t="s">
         <v>10656</v>
       </c>
-      <c r="AK64" s="0" t="s">
-        <v>10653</v>
-      </c>
-      <c r="AL64" s="0" t="s">
+      <c r="AV64" s="0" t="s">
         <v>10657</v>
-      </c>
-      <c r="AM64" s="0" t="s">
-        <v>10654</v>
-      </c>
-      <c r="AN64" s="0" t="s">
-        <v>10658</v>
-      </c>
-      <c r="AO64" s="0" t="s">
-        <v>10659</v>
-      </c>
-      <c r="AP64" s="0" t="s">
-        <v>10660</v>
-      </c>
-      <c r="AQ64" s="0" t="s">
-        <v>10661</v>
-      </c>
-      <c r="AR64" s="0" t="s">
-        <v>10662</v>
-      </c>
-      <c r="AS64" s="0" t="s">
-        <v>10663</v>
-      </c>
-      <c r="AT64" s="0" t="s">
-        <v>10664</v>
-      </c>
-      <c r="AU64" s="0" t="s">
-        <v>10665</v>
-      </c>
-      <c r="AV64" s="0" t="s">
-        <v>10666</v>
       </c>
       <c r="AW64" s="0" t="s">
         <v>10305</v>
       </c>
       <c r="AX64" s="0" t="s">
+        <v>10658</v>
+      </c>
+      <c r="AY64" s="0" t="s">
+        <v>10659</v>
+      </c>
+      <c r="AZ64" s="0" t="s">
+        <v>10660</v>
+      </c>
+      <c r="BA64" s="0" t="s">
+        <v>10661</v>
+      </c>
+      <c r="BB64" s="0" t="s">
+        <v>10662</v>
+      </c>
+      <c r="BC64" s="0" t="s">
+        <v>10663</v>
+      </c>
+      <c r="BD64" s="0" t="s">
+        <v>10664</v>
+      </c>
+      <c r="BE64" s="0" t="s">
+        <v>10665</v>
+      </c>
+      <c r="BF64" s="0" t="s">
+        <v>10666</v>
+      </c>
+      <c r="BG64" s="0" t="s">
         <v>10667</v>
       </c>
-      <c r="AY64" s="0" t="s">
+      <c r="BH64" s="0" t="s">
         <v>10668</v>
       </c>
-      <c r="AZ64" s="0" t="s">
+      <c r="BI64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="BJ64" s="0" t="s">
         <v>10669</v>
       </c>
-      <c r="BA64" s="0" t="s">
+      <c r="BK64" s="0" t="s">
         <v>10670</v>
       </c>
-      <c r="BB64" s="0" t="s">
+      <c r="BL64" s="0" t="s">
         <v>10671</v>
       </c>
-      <c r="BC64" s="0" t="s">
+      <c r="BM64" s="0" t="s">
         <v>10672</v>
       </c>
-      <c r="BD64" s="0" t="s">
+      <c r="BN64" s="0" t="s">
         <v>10673</v>
-      </c>
-      <c r="BE64" s="0" t="s">
-        <v>10674</v>
-      </c>
-      <c r="BF64" s="0" t="s">
-        <v>10675</v>
-      </c>
-      <c r="BG64" s="0" t="s">
-        <v>10676</v>
-      </c>
-      <c r="BH64" s="0" t="s">
-        <v>10677</v>
-      </c>
-      <c r="BI64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="BJ64" s="0" t="s">
-        <v>10678</v>
-      </c>
-      <c r="BK64" s="0" t="s">
-        <v>10679</v>
-      </c>
-      <c r="BL64" s="0" t="s">
-        <v>10680</v>
-      </c>
-      <c r="BM64" s="0" t="s">
-        <v>10681</v>
-      </c>
-      <c r="BN64" s="0" t="s">
-        <v>10682</v>
       </c>
       <c r="BO64" s="0" t="s">
         <v>310</v>
@@ -78556,166 +78536,166 @@
         <v>310</v>
       </c>
       <c r="BR64" s="0" t="s">
+        <v>10674</v>
+      </c>
+      <c r="BS64" s="0" t="s">
+        <v>10675</v>
+      </c>
+      <c r="BT64" s="0" t="s">
+        <v>10676</v>
+      </c>
+      <c r="BU64" s="0" t="s">
+        <v>10677</v>
+      </c>
+      <c r="BV64" s="0" t="s">
+        <v>10678</v>
+      </c>
+      <c r="BW64" s="0" t="s">
+        <v>10679</v>
+      </c>
+      <c r="BX64" s="0" t="s">
+        <v>10680</v>
+      </c>
+      <c r="BY64" s="0" t="s">
+        <v>10681</v>
+      </c>
+      <c r="BZ64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CA64" s="0" t="s">
+        <v>10682</v>
+      </c>
+      <c r="CB64" s="0" t="s">
         <v>10683</v>
       </c>
-      <c r="BS64" s="0" t="s">
+      <c r="CC64" s="0" t="s">
         <v>10684</v>
       </c>
-      <c r="BT64" s="0" t="s">
+      <c r="CD64" s="0" t="s">
         <v>10685</v>
       </c>
-      <c r="BU64" s="0" t="s">
+      <c r="CE64" s="0" t="s">
         <v>10686</v>
       </c>
-      <c r="BV64" s="0" t="s">
+      <c r="CF64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CG64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CH64" s="0" t="s">
         <v>10687</v>
       </c>
-      <c r="BW64" s="0" t="s">
+      <c r="CI64" s="0" t="s">
         <v>10688</v>
       </c>
-      <c r="BX64" s="0" t="s">
+      <c r="CJ64" s="0" t="s">
         <v>10689</v>
       </c>
-      <c r="BY64" s="0" t="s">
+      <c r="CK64" s="0" t="s">
         <v>10690</v>
       </c>
-      <c r="BZ64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CA64" s="0" t="s">
+      <c r="CL64" s="0" t="s">
         <v>10691</v>
       </c>
-      <c r="CB64" s="0" t="s">
+      <c r="CM64" s="0" t="s">
         <v>10692</v>
       </c>
-      <c r="CC64" s="0" t="s">
+      <c r="CN64" s="0" t="s">
         <v>10693</v>
       </c>
-      <c r="CD64" s="0" t="s">
+      <c r="CO64" s="0" t="s">
         <v>10694</v>
       </c>
-      <c r="CE64" s="0" t="s">
+      <c r="CP64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CQ64" s="0" t="s">
         <v>10695</v>
       </c>
-      <c r="CF64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CG64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CH64" s="0" t="s">
+      <c r="CR64" s="0" t="s">
         <v>10696</v>
       </c>
-      <c r="CI64" s="0" t="s">
+      <c r="CS64" s="0" t="s">
         <v>10697</v>
       </c>
-      <c r="CJ64" s="0" t="s">
+      <c r="CT64" s="0" t="s">
         <v>10698</v>
       </c>
-      <c r="CK64" s="0" t="s">
+      <c r="CU64" s="0" t="s">
         <v>10699</v>
       </c>
-      <c r="CL64" s="0" t="s">
+      <c r="CV64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CW64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="CX64" s="0" t="s">
         <v>10700</v>
       </c>
-      <c r="CM64" s="0" t="s">
+      <c r="CY64" s="0" t="s">
         <v>10701</v>
       </c>
-      <c r="CN64" s="0" t="s">
+      <c r="CZ64" s="0" t="s">
         <v>10702</v>
       </c>
-      <c r="CO64" s="0" t="s">
+      <c r="DA64" s="0" t="s">
         <v>10703</v>
       </c>
-      <c r="CP64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CQ64" s="0" t="s">
+      <c r="DB64" s="0" t="s">
         <v>10704</v>
       </c>
-      <c r="CR64" s="0" t="s">
+      <c r="DC64" s="0" t="s">
         <v>10705</v>
       </c>
-      <c r="CS64" s="0" t="s">
+      <c r="DD64" s="0" t="s">
         <v>10706</v>
       </c>
-      <c r="CT64" s="0" t="s">
+      <c r="DE64" s="0" t="s">
         <v>10707</v>
       </c>
-      <c r="CU64" s="0" t="s">
+      <c r="DF64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG64" s="0" t="s">
         <v>10708</v>
       </c>
-      <c r="CV64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CW64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="CX64" s="0" t="s">
+      <c r="DH64" s="0" t="s">
         <v>10709</v>
       </c>
-      <c r="CY64" s="0" t="s">
+      <c r="DI64" s="0" t="s">
         <v>10710</v>
       </c>
-      <c r="CZ64" s="0" t="s">
+      <c r="DJ64" s="0" t="s">
         <v>10711</v>
       </c>
-      <c r="DA64" s="0" t="s">
+      <c r="DK64" s="0" t="s">
         <v>10712</v>
       </c>
-      <c r="DB64" s="0" t="s">
+      <c r="DL64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DN64" s="0" t="s">
         <v>10713</v>
       </c>
-      <c r="DC64" s="0" t="s">
+      <c r="DO64" s="0" t="s">
         <v>10714</v>
       </c>
-      <c r="DD64" s="0" t="s">
+      <c r="DP64" s="0" t="s">
         <v>10715</v>
       </c>
-      <c r="DE64" s="0" t="s">
+      <c r="DQ64" s="0" t="s">
         <v>10716</v>
       </c>
-      <c r="DF64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG64" s="0" t="s">
+      <c r="DR64" s="0" t="s">
         <v>10717</v>
       </c>
-      <c r="DH64" s="0" t="s">
+      <c r="DS64" s="0" t="s">
         <v>10718</v>
-      </c>
-      <c r="DI64" s="0" t="s">
-        <v>10719</v>
-      </c>
-      <c r="DJ64" s="0" t="s">
-        <v>10720</v>
-      </c>
-      <c r="DK64" s="0" t="s">
-        <v>10721</v>
-      </c>
-      <c r="DL64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DN64" s="0" t="s">
-        <v>10722</v>
-      </c>
-      <c r="DO64" s="0" t="s">
-        <v>10723</v>
-      </c>
-      <c r="DP64" s="0" t="s">
-        <v>10724</v>
-      </c>
-      <c r="DQ64" s="0" t="s">
-        <v>10725</v>
-      </c>
-      <c r="DR64" s="0" t="s">
-        <v>10726</v>
-      </c>
-      <c r="DS64" s="0" t="s">
-        <v>10727</v>
       </c>
       <c r="DT64" s="0" t="s">
         <v>885</v>
@@ -78724,19 +78704,19 @@
         <v>7281</v>
       </c>
       <c r="DV64" s="0" t="s">
-        <v>10728</v>
+        <v>10719</v>
       </c>
       <c r="DW64" s="0" t="s">
-        <v>10729</v>
+        <v>10720</v>
       </c>
       <c r="DY64" s="0" t="s">
-        <v>10730</v>
+        <v>10721</v>
       </c>
       <c r="DZ64" s="0" t="s">
-        <v>10731</v>
+        <v>10722</v>
       </c>
       <c r="EA64" s="0" t="s">
-        <v>10732</v>
+        <v>10723</v>
       </c>
       <c r="EB64" s="0" t="s">
         <v>310</v>
@@ -78745,55 +78725,55 @@
         <v>370</v>
       </c>
       <c r="ED64" s="0" t="s">
+        <v>10721</v>
+      </c>
+      <c r="EE64" s="0" t="s">
+        <v>10724</v>
+      </c>
+      <c r="EF64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="EG64" s="0" t="s">
+        <v>10725</v>
+      </c>
+      <c r="EH64" s="0" t="s">
+        <v>10726</v>
+      </c>
+      <c r="EI64" s="0" t="s">
+        <v>10727</v>
+      </c>
+      <c r="EJ64" s="0" t="s">
+        <v>10728</v>
+      </c>
+      <c r="EK64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="EL64" s="0" t="s">
+        <v>10729</v>
+      </c>
+      <c r="EM64" s="0" t="s">
         <v>10730</v>
       </c>
-      <c r="EE64" s="0" t="s">
-        <v>10733</v>
-      </c>
-      <c r="EF64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="EG64" s="0" t="s">
-        <v>10734</v>
-      </c>
-      <c r="EH64" s="0" t="s">
-        <v>10735</v>
-      </c>
-      <c r="EI64" s="0" t="s">
-        <v>10736</v>
-      </c>
-      <c r="EJ64" s="0" t="s">
-        <v>10737</v>
-      </c>
-      <c r="EK64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="EL64" s="0" t="s">
-        <v>10738</v>
-      </c>
-      <c r="EM64" s="0" t="s">
-        <v>10739</v>
-      </c>
       <c r="EN64" s="0" t="s">
-        <v>10740</v>
+        <v>10731</v>
       </c>
       <c r="EP64" s="0" t="s">
         <v>1274</v>
       </c>
       <c r="EQ64" s="0" t="s">
-        <v>10741</v>
+        <v>10732</v>
       </c>
       <c r="ES64" s="0" t="s">
-        <v>10742</v>
+        <v>10733</v>
       </c>
       <c r="EV64" s="0" t="s">
-        <v>10743</v>
+        <v>10734</v>
       </c>
       <c r="EW64" s="0" t="s">
-        <v>10744</v>
+        <v>10735</v>
       </c>
       <c r="EX64" s="0" t="s">
-        <v>10745</v>
+        <v>10736</v>
       </c>
       <c r="EY64" s="0" t="s">
         <v>310</v>
@@ -78802,61 +78782,61 @@
         <v>370</v>
       </c>
       <c r="FA64" s="0" t="s">
+        <v>10734</v>
+      </c>
+      <c r="FB64" s="0" t="s">
+        <v>10737</v>
+      </c>
+      <c r="FC64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="FD64" s="0" t="s">
+        <v>10738</v>
+      </c>
+      <c r="FE64" s="0" t="s">
+        <v>10739</v>
+      </c>
+      <c r="FF64" s="0" t="s">
+        <v>10740</v>
+      </c>
+      <c r="FG64" s="0" t="s">
+        <v>10741</v>
+      </c>
+      <c r="FH64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="FI64" s="0" t="s">
+        <v>10742</v>
+      </c>
+      <c r="FJ64" s="0" t="s">
         <v>10743</v>
       </c>
-      <c r="FB64" s="0" t="s">
-        <v>10746</v>
-      </c>
-      <c r="FC64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="FD64" s="0" t="s">
-        <v>10747</v>
-      </c>
-      <c r="FE64" s="0" t="s">
-        <v>10748</v>
-      </c>
-      <c r="FF64" s="0" t="s">
-        <v>10749</v>
-      </c>
-      <c r="FG64" s="0" t="s">
-        <v>10750</v>
-      </c>
-      <c r="FH64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="FI64" s="0" t="s">
-        <v>10751</v>
-      </c>
-      <c r="FJ64" s="0" t="s">
-        <v>10752</v>
-      </c>
       <c r="FK64" s="0" t="s">
-        <v>10753</v>
+        <v>10744</v>
       </c>
       <c r="FM64" s="0" t="s">
         <v>399</v>
       </c>
       <c r="FN64" s="0" t="s">
-        <v>10754</v>
+        <v>10745</v>
       </c>
       <c r="FO64" s="0" t="s">
         <v>580</v>
       </c>
       <c r="FP64" s="0" t="s">
-        <v>10755</v>
+        <v>10746</v>
       </c>
       <c r="FQ64" s="0" t="s">
         <v>3255</v>
       </c>
       <c r="FS64" s="0" t="s">
-        <v>10756</v>
+        <v>10747</v>
       </c>
       <c r="FT64" s="0" t="s">
-        <v>10757</v>
+        <v>10748</v>
       </c>
       <c r="FU64" s="0" t="s">
-        <v>10758</v>
+        <v>10749</v>
       </c>
       <c r="FV64" s="0" t="s">
         <v>310</v>
@@ -78865,61 +78845,61 @@
         <v>370</v>
       </c>
       <c r="FX64" s="0" t="s">
+        <v>10747</v>
+      </c>
+      <c r="FY64" s="0" t="s">
+        <v>10750</v>
+      </c>
+      <c r="FZ64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GA64" s="0" t="s">
+        <v>10751</v>
+      </c>
+      <c r="GB64" s="0" t="s">
+        <v>10752</v>
+      </c>
+      <c r="GC64" s="0" t="s">
+        <v>10753</v>
+      </c>
+      <c r="GD64" s="0" t="s">
+        <v>10754</v>
+      </c>
+      <c r="GE64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GF64" s="0" t="s">
+        <v>10755</v>
+      </c>
+      <c r="GG64" s="0" t="s">
         <v>10756</v>
       </c>
-      <c r="FY64" s="0" t="s">
-        <v>10759</v>
-      </c>
-      <c r="FZ64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GA64" s="0" t="s">
-        <v>10760</v>
-      </c>
-      <c r="GB64" s="0" t="s">
-        <v>10761</v>
-      </c>
-      <c r="GC64" s="0" t="s">
-        <v>10762</v>
-      </c>
-      <c r="GD64" s="0" t="s">
-        <v>10763</v>
-      </c>
-      <c r="GE64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GF64" s="0" t="s">
-        <v>10764</v>
-      </c>
-      <c r="GG64" s="0" t="s">
-        <v>10765</v>
-      </c>
       <c r="GH64" s="0" t="s">
-        <v>10766</v>
+        <v>10757</v>
       </c>
       <c r="GJ64" s="0" t="s">
         <v>4186</v>
       </c>
       <c r="GL64" s="0" t="s">
-        <v>10767</v>
+        <v>10758</v>
       </c>
       <c r="GM64" s="0" t="s">
         <v>2714</v>
       </c>
       <c r="GN64" s="0" t="s">
-        <v>10768</v>
+        <v>10759</v>
       </c>
       <c r="GO64" s="0" t="s">
-        <v>10769</v>
+        <v>10760</v>
       </c>
       <c r="GQ64" s="0" t="s">
-        <v>10770</v>
+        <v>10761</v>
       </c>
       <c r="GR64" s="0" t="s">
-        <v>10771</v>
+        <v>10762</v>
       </c>
       <c r="GS64" s="0" t="s">
-        <v>10772</v>
+        <v>10763</v>
       </c>
       <c r="GT64" s="0" t="s">
         <v>310</v>
@@ -78928,231 +78908,231 @@
         <v>370</v>
       </c>
       <c r="GV64" s="0" t="s">
+        <v>10761</v>
+      </c>
+      <c r="GW64" s="0" t="s">
+        <v>10764</v>
+      </c>
+      <c r="GX64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GY64" s="0" t="s">
+        <v>10765</v>
+      </c>
+      <c r="GZ64" s="0" t="s">
+        <v>10766</v>
+      </c>
+      <c r="HA64" s="0" t="s">
+        <v>10767</v>
+      </c>
+      <c r="HB64" s="0" t="s">
+        <v>10768</v>
+      </c>
+      <c r="HC64" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="HD64" s="0" t="s">
+        <v>10769</v>
+      </c>
+      <c r="HE64" s="0" t="s">
         <v>10770</v>
       </c>
-      <c r="GW64" s="0" t="s">
+      <c r="HF64" s="0" t="s">
+        <v>10771</v>
+      </c>
+      <c r="HG64" s="0" t="s">
+        <v>10772</v>
+      </c>
+      <c r="HH64" s="0" t="s">
         <v>10773</v>
       </c>
-      <c r="GX64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GY64" s="0" t="s">
+      <c r="HI64" s="0" t="s">
         <v>10774</v>
       </c>
-      <c r="GZ64" s="0" t="s">
+      <c r="HJ64" s="0" t="s">
         <v>10775</v>
       </c>
-      <c r="HA64" s="0" t="s">
+      <c r="HK64" s="0" t="s">
         <v>10776</v>
       </c>
-      <c r="HB64" s="0" t="s">
+      <c r="HL64" s="0" t="s">
         <v>10777</v>
       </c>
-      <c r="HC64" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="HD64" s="0" t="s">
+      <c r="HM64" s="0" t="s">
         <v>10778</v>
       </c>
-      <c r="HE64" s="0" t="s">
+      <c r="HN64" s="0" t="s">
         <v>10779</v>
       </c>
-      <c r="HF64" s="0" t="s">
+      <c r="HO64" s="0" t="s">
         <v>10780</v>
       </c>
-      <c r="HG64" s="0" t="s">
+      <c r="HP64" s="0" t="s">
         <v>10781</v>
-      </c>
-      <c r="HH64" s="0" t="s">
-        <v>10782</v>
-      </c>
-      <c r="HI64" s="0" t="s">
-        <v>10783</v>
-      </c>
-      <c r="HJ64" s="0" t="s">
-        <v>10784</v>
-      </c>
-      <c r="HK64" s="0" t="s">
-        <v>10785</v>
-      </c>
-      <c r="HL64" s="0" t="s">
-        <v>10786</v>
-      </c>
-      <c r="HM64" s="0" t="s">
-        <v>10787</v>
-      </c>
-      <c r="HN64" s="0" t="s">
-        <v>10788</v>
-      </c>
-      <c r="HO64" s="0" t="s">
-        <v>10789</v>
-      </c>
-      <c r="HP64" s="0" t="s">
-        <v>10790</v>
       </c>
       <c r="HQ64" s="0" t="s">
         <v>414</v>
       </c>
       <c r="HR64" s="0" t="s">
-        <v>10791</v>
+        <v>10782</v>
       </c>
       <c r="HS64" s="0" t="s">
         <v>2707</v>
       </c>
       <c r="HT64" s="0" t="s">
+        <v>10783</v>
+      </c>
+      <c r="HU64" s="0" t="s">
+        <v>10784</v>
+      </c>
+      <c r="HV64" s="0" t="s">
+        <v>10785</v>
+      </c>
+      <c r="HW64" s="0" t="s">
+        <v>10786</v>
+      </c>
+      <c r="HX64" s="0" t="s">
+        <v>10787</v>
+      </c>
+      <c r="HY64" s="0" t="s">
+        <v>10788</v>
+      </c>
+      <c r="HZ64" s="0" t="s">
+        <v>10789</v>
+      </c>
+      <c r="IA64" s="0" t="s">
+        <v>10790</v>
+      </c>
+      <c r="IB64" s="0" t="s">
+        <v>10600</v>
+      </c>
+      <c r="IC64" s="0" t="s">
+        <v>10791</v>
+      </c>
+      <c r="ID64" s="0" t="s">
         <v>10792</v>
       </c>
-      <c r="HU64" s="0" t="s">
+      <c r="IE64" s="0" t="s">
         <v>10793</v>
       </c>
-      <c r="HV64" s="0" t="s">
+      <c r="IF64" s="0" t="s">
         <v>10794</v>
       </c>
-      <c r="HW64" s="0" t="s">
+      <c r="IG64" s="0" t="s">
         <v>10795</v>
       </c>
-      <c r="HX64" s="0" t="s">
+      <c r="IH64" s="0" t="s">
         <v>10796</v>
       </c>
-      <c r="HY64" s="0" t="s">
+      <c r="II64" s="0" t="s">
         <v>10797</v>
       </c>
-      <c r="HZ64" s="0" t="s">
+      <c r="IJ64" s="0" t="s">
         <v>10798</v>
       </c>
-      <c r="IA64" s="0" t="s">
+      <c r="IK64" s="0" t="s">
         <v>10799</v>
       </c>
-      <c r="IB64" s="0" t="s">
-        <v>10605</v>
-      </c>
-      <c r="IC64" s="0" t="s">
+      <c r="IL64" s="0" t="s">
         <v>10800</v>
       </c>
-      <c r="ID64" s="0" t="s">
+      <c r="IM64" s="0" t="s">
         <v>10801</v>
       </c>
-      <c r="IE64" s="0" t="s">
+      <c r="IN64" s="0" t="s">
         <v>10802</v>
       </c>
-      <c r="IF64" s="0" t="s">
+      <c r="IO64" s="0" t="s">
         <v>10803</v>
       </c>
-      <c r="IG64" s="0" t="s">
+      <c r="IP64" s="0" t="s">
         <v>10804</v>
       </c>
-      <c r="IH64" s="0" t="s">
+      <c r="IQ64" s="0" t="s">
         <v>10805</v>
-      </c>
-      <c r="II64" s="0" t="s">
-        <v>10806</v>
-      </c>
-      <c r="IJ64" s="0" t="s">
-        <v>10807</v>
-      </c>
-      <c r="IK64" s="0" t="s">
-        <v>10808</v>
-      </c>
-      <c r="IL64" s="0" t="s">
-        <v>10809</v>
-      </c>
-      <c r="IM64" s="0" t="s">
-        <v>10810</v>
-      </c>
-      <c r="IN64" s="0" t="s">
-        <v>10811</v>
-      </c>
-      <c r="IO64" s="0" t="s">
-        <v>10812</v>
-      </c>
-      <c r="IP64" s="0" t="s">
-        <v>10813</v>
-      </c>
-      <c r="IQ64" s="0" t="s">
-        <v>10814</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX65" s="0" t="s">
+        <v>10806</v>
+      </c>
+      <c r="CY65" s="0" t="s">
+        <v>10807</v>
+      </c>
+      <c r="CZ65" s="0" t="s">
+        <v>10808</v>
+      </c>
+      <c r="DA65" s="0" t="s">
+        <v>10809</v>
+      </c>
+      <c r="DB65" s="0" t="s">
+        <v>10810</v>
+      </c>
+      <c r="DC65" s="0" t="s">
+        <v>10811</v>
+      </c>
+      <c r="DD65" s="0" t="s">
+        <v>10812</v>
+      </c>
+      <c r="DE65" s="0" t="s">
+        <v>10813</v>
+      </c>
+      <c r="DF65" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG65" s="0" t="s">
+        <v>10814</v>
+      </c>
+      <c r="DH65" s="0" t="s">
         <v>10815</v>
       </c>
-      <c r="CY65" s="0" t="s">
+      <c r="DI65" s="0" t="s">
         <v>10816</v>
       </c>
-      <c r="CZ65" s="0" t="s">
+      <c r="DJ65" s="0" t="s">
         <v>10817</v>
       </c>
-      <c r="DA65" s="0" t="s">
+      <c r="DK65" s="0" t="s">
         <v>10818</v>
       </c>
-      <c r="DB65" s="0" t="s">
+      <c r="DL65" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM65" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE65" s="0" t="s">
         <v>10819</v>
       </c>
-      <c r="DC65" s="0" t="s">
+      <c r="GF65" s="0" t="s">
         <v>10820</v>
       </c>
-      <c r="DD65" s="0" t="s">
+      <c r="GG65" s="0" t="s">
         <v>10821</v>
       </c>
-      <c r="DE65" s="0" t="s">
+      <c r="GI65" s="0" t="s">
         <v>10822</v>
       </c>
-      <c r="DF65" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG65" s="0" t="s">
+      <c r="GJ65" s="0" t="s">
         <v>10823</v>
       </c>
-      <c r="DH65" s="0" t="s">
+      <c r="GK65" s="0" t="s">
         <v>10824</v>
       </c>
-      <c r="DI65" s="0" t="s">
+      <c r="GL65" s="0" t="s">
         <v>10825</v>
-      </c>
-      <c r="DJ65" s="0" t="s">
-        <v>10826</v>
-      </c>
-      <c r="DK65" s="0" t="s">
-        <v>10827</v>
-      </c>
-      <c r="DL65" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM65" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE65" s="0" t="s">
-        <v>10828</v>
-      </c>
-      <c r="GF65" s="0" t="s">
-        <v>10829</v>
-      </c>
-      <c r="GG65" s="0" t="s">
-        <v>10830</v>
-      </c>
-      <c r="GI65" s="0" t="s">
-        <v>10831</v>
-      </c>
-      <c r="GJ65" s="0" t="s">
-        <v>10832</v>
-      </c>
-      <c r="GK65" s="0" t="s">
-        <v>10833</v>
-      </c>
-      <c r="GL65" s="0" t="s">
-        <v>10834</v>
       </c>
       <c r="GM65" s="0" t="s">
         <v>5854</v>
       </c>
       <c r="GO65" s="0" t="s">
-        <v>10835</v>
+        <v>10826</v>
       </c>
       <c r="GP65" s="0" t="s">
-        <v>10836</v>
+        <v>10827</v>
       </c>
       <c r="GQ65" s="0" t="s">
-        <v>10837</v>
+        <v>10828</v>
       </c>
       <c r="GR65" s="0" t="s">
         <v>310</v>
@@ -79161,129 +79141,129 @@
         <v>370</v>
       </c>
       <c r="GT65" s="0" t="s">
+        <v>10829</v>
+      </c>
+      <c r="GU65" s="0" t="s">
+        <v>10830</v>
+      </c>
+      <c r="GV65" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW65" s="0" t="s">
+        <v>10831</v>
+      </c>
+      <c r="GX65" s="0" t="s">
+        <v>10832</v>
+      </c>
+      <c r="GY65" s="0" t="s">
+        <v>10833</v>
+      </c>
+      <c r="GZ65" s="0" t="s">
+        <v>10834</v>
+      </c>
+      <c r="HA65" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC65" s="0" t="s">
+        <v>10835</v>
+      </c>
+      <c r="ID65" s="0" t="s">
+        <v>10836</v>
+      </c>
+      <c r="IE65" s="0" t="s">
+        <v>10837</v>
+      </c>
+      <c r="IF65" s="0" t="s">
         <v>10838</v>
       </c>
-      <c r="GU65" s="0" t="s">
+      <c r="IG65" s="0" t="s">
         <v>10839</v>
       </c>
-      <c r="GV65" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW65" s="0" t="s">
+      <c r="IH65" s="0" t="s">
         <v>10840</v>
       </c>
-      <c r="GX65" s="0" t="s">
+      <c r="II65" s="0" t="s">
         <v>10841</v>
       </c>
-      <c r="GY65" s="0" t="s">
+      <c r="IJ65" s="0" t="s">
         <v>10842</v>
       </c>
-      <c r="GZ65" s="0" t="s">
+      <c r="IK65" s="0" t="s">
         <v>10843</v>
-      </c>
-      <c r="HA65" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC65" s="0" t="s">
-        <v>10844</v>
-      </c>
-      <c r="ID65" s="0" t="s">
-        <v>10845</v>
-      </c>
-      <c r="IE65" s="0" t="s">
-        <v>10846</v>
-      </c>
-      <c r="IF65" s="0" t="s">
-        <v>10847</v>
-      </c>
-      <c r="IG65" s="0" t="s">
-        <v>10848</v>
-      </c>
-      <c r="IH65" s="0" t="s">
-        <v>10849</v>
-      </c>
-      <c r="II65" s="0" t="s">
-        <v>10850</v>
-      </c>
-      <c r="IJ65" s="0" t="s">
-        <v>10851</v>
-      </c>
-      <c r="IK65" s="0" t="s">
-        <v>10852</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX66" s="0" t="s">
+        <v>10844</v>
+      </c>
+      <c r="CY66" s="0" t="s">
+        <v>10845</v>
+      </c>
+      <c r="CZ66" s="0" t="s">
+        <v>10846</v>
+      </c>
+      <c r="DA66" s="0" t="s">
+        <v>10847</v>
+      </c>
+      <c r="DB66" s="0" t="s">
+        <v>10848</v>
+      </c>
+      <c r="DC66" s="0" t="s">
+        <v>10849</v>
+      </c>
+      <c r="DD66" s="0" t="s">
+        <v>10850</v>
+      </c>
+      <c r="DE66" s="0" t="s">
+        <v>10851</v>
+      </c>
+      <c r="DF66" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG66" s="0" t="s">
+        <v>10852</v>
+      </c>
+      <c r="DH66" s="0" t="s">
         <v>10853</v>
       </c>
-      <c r="CY66" s="0" t="s">
+      <c r="DI66" s="0" t="s">
         <v>10854</v>
       </c>
-      <c r="CZ66" s="0" t="s">
+      <c r="DJ66" s="0" t="s">
         <v>10855</v>
       </c>
-      <c r="DA66" s="0" t="s">
+      <c r="DK66" s="0" t="s">
         <v>10856</v>
       </c>
-      <c r="DB66" s="0" t="s">
+      <c r="DL66" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM66" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE66" s="0" t="s">
         <v>10857</v>
       </c>
-      <c r="DC66" s="0" t="s">
+      <c r="GF66" s="0" t="s">
         <v>10858</v>
       </c>
-      <c r="DD66" s="0" t="s">
+      <c r="GG66" s="0" t="s">
         <v>10859</v>
       </c>
-      <c r="DE66" s="0" t="s">
+      <c r="GJ66" s="0" t="s">
         <v>10860</v>
       </c>
-      <c r="DF66" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG66" s="0" t="s">
+      <c r="GL66" s="0" t="s">
         <v>10861</v>
       </c>
-      <c r="DH66" s="0" t="s">
+      <c r="GO66" s="0" t="s">
         <v>10862</v>
       </c>
-      <c r="DI66" s="0" t="s">
+      <c r="GP66" s="0" t="s">
         <v>10863</v>
       </c>
-      <c r="DJ66" s="0" t="s">
+      <c r="GQ66" s="0" t="s">
         <v>10864</v>
-      </c>
-      <c r="DK66" s="0" t="s">
-        <v>10865</v>
-      </c>
-      <c r="DL66" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM66" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE66" s="0" t="s">
-        <v>10866</v>
-      </c>
-      <c r="GF66" s="0" t="s">
-        <v>10867</v>
-      </c>
-      <c r="GG66" s="0" t="s">
-        <v>10868</v>
-      </c>
-      <c r="GJ66" s="0" t="s">
-        <v>10869</v>
-      </c>
-      <c r="GL66" s="0" t="s">
-        <v>10870</v>
-      </c>
-      <c r="GO66" s="0" t="s">
-        <v>10871</v>
-      </c>
-      <c r="GP66" s="0" t="s">
-        <v>10872</v>
-      </c>
-      <c r="GQ66" s="0" t="s">
-        <v>10873</v>
       </c>
       <c r="GR66" s="0" t="s">
         <v>310</v>
@@ -79292,126 +79272,126 @@
         <v>370</v>
       </c>
       <c r="GT66" s="0" t="s">
-        <v>10835</v>
+        <v>10826</v>
       </c>
       <c r="GU66" s="0" t="s">
+        <v>10865</v>
+      </c>
+      <c r="GV66" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW66" s="0" t="s">
+        <v>10866</v>
+      </c>
+      <c r="GX66" s="0" t="s">
+        <v>10867</v>
+      </c>
+      <c r="GY66" s="0" t="s">
+        <v>10868</v>
+      </c>
+      <c r="GZ66" s="0" t="s">
+        <v>10869</v>
+      </c>
+      <c r="HA66" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC66" s="0" t="s">
+        <v>10870</v>
+      </c>
+      <c r="ID66" s="0" t="s">
+        <v>10871</v>
+      </c>
+      <c r="IE66" s="0" t="s">
+        <v>10872</v>
+      </c>
+      <c r="IF66" s="0" t="s">
+        <v>10873</v>
+      </c>
+      <c r="IG66" s="0" t="s">
         <v>10874</v>
       </c>
-      <c r="GV66" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW66" s="0" t="s">
+      <c r="IH66" s="0" t="s">
         <v>10875</v>
       </c>
-      <c r="GX66" s="0" t="s">
+      <c r="IJ66" s="0" t="s">
         <v>10876</v>
       </c>
-      <c r="GY66" s="0" t="s">
+      <c r="IK66" s="0" t="s">
         <v>10877</v>
-      </c>
-      <c r="GZ66" s="0" t="s">
-        <v>10878</v>
-      </c>
-      <c r="HA66" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC66" s="0" t="s">
-        <v>10879</v>
-      </c>
-      <c r="ID66" s="0" t="s">
-        <v>10880</v>
-      </c>
-      <c r="IE66" s="0" t="s">
-        <v>10881</v>
-      </c>
-      <c r="IF66" s="0" t="s">
-        <v>10882</v>
-      </c>
-      <c r="IG66" s="0" t="s">
-        <v>10883</v>
-      </c>
-      <c r="IH66" s="0" t="s">
-        <v>10884</v>
-      </c>
-      <c r="IJ66" s="0" t="s">
-        <v>10885</v>
-      </c>
-      <c r="IK66" s="0" t="s">
-        <v>10886</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX67" s="0" t="s">
+        <v>10878</v>
+      </c>
+      <c r="CY67" s="0" t="s">
+        <v>10879</v>
+      </c>
+      <c r="CZ67" s="0" t="s">
+        <v>10880</v>
+      </c>
+      <c r="DA67" s="0" t="s">
+        <v>10881</v>
+      </c>
+      <c r="DB67" s="0" t="s">
+        <v>10882</v>
+      </c>
+      <c r="DC67" s="0" t="s">
+        <v>10883</v>
+      </c>
+      <c r="DD67" s="0" t="s">
+        <v>10884</v>
+      </c>
+      <c r="DE67" s="0" t="s">
+        <v>10885</v>
+      </c>
+      <c r="DF67" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG67" s="0" t="s">
+        <v>10886</v>
+      </c>
+      <c r="DH67" s="0" t="s">
         <v>10887</v>
       </c>
-      <c r="CY67" s="0" t="s">
+      <c r="DI67" s="0" t="s">
         <v>10888</v>
       </c>
-      <c r="CZ67" s="0" t="s">
+      <c r="DJ67" s="0" t="s">
         <v>10889</v>
       </c>
-      <c r="DA67" s="0" t="s">
+      <c r="DK67" s="0" t="s">
         <v>10890</v>
       </c>
-      <c r="DB67" s="0" t="s">
+      <c r="DL67" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM67" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE67" s="0" t="s">
         <v>10891</v>
       </c>
-      <c r="DC67" s="0" t="s">
+      <c r="GF67" s="0" t="s">
         <v>10892</v>
       </c>
-      <c r="DD67" s="0" t="s">
+      <c r="GG67" s="0" t="s">
         <v>10893</v>
       </c>
-      <c r="DE67" s="0" t="s">
+      <c r="GJ67" s="0" t="s">
         <v>10894</v>
       </c>
-      <c r="DF67" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG67" s="0" t="s">
+      <c r="GL67" s="0" t="s">
         <v>10895</v>
       </c>
-      <c r="DH67" s="0" t="s">
+      <c r="GO67" s="0" t="s">
         <v>10896</v>
       </c>
-      <c r="DI67" s="0" t="s">
+      <c r="GP67" s="0" t="s">
         <v>10897</v>
       </c>
-      <c r="DJ67" s="0" t="s">
+      <c r="GQ67" s="0" t="s">
         <v>10898</v>
-      </c>
-      <c r="DK67" s="0" t="s">
-        <v>10899</v>
-      </c>
-      <c r="DL67" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM67" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE67" s="0" t="s">
-        <v>10900</v>
-      </c>
-      <c r="GF67" s="0" t="s">
-        <v>10901</v>
-      </c>
-      <c r="GG67" s="0" t="s">
-        <v>10902</v>
-      </c>
-      <c r="GJ67" s="0" t="s">
-        <v>10903</v>
-      </c>
-      <c r="GL67" s="0" t="s">
-        <v>10904</v>
-      </c>
-      <c r="GO67" s="0" t="s">
-        <v>10905</v>
-      </c>
-      <c r="GP67" s="0" t="s">
-        <v>10906</v>
-      </c>
-      <c r="GQ67" s="0" t="s">
-        <v>10907</v>
       </c>
       <c r="GR67" s="0" t="s">
         <v>310</v>
@@ -79420,49 +79400,49 @@
         <v>370</v>
       </c>
       <c r="GT67" s="0" t="s">
-        <v>10871</v>
+        <v>10862</v>
       </c>
       <c r="GU67" s="0" t="s">
-        <v>10908</v>
+        <v>10899</v>
       </c>
       <c r="GV67" s="0" t="s">
         <v>310</v>
       </c>
       <c r="GW67" s="0" t="s">
-        <v>10909</v>
+        <v>10900</v>
       </c>
       <c r="GX67" s="0" t="s">
-        <v>10910</v>
+        <v>10901</v>
       </c>
       <c r="GY67" s="0" t="s">
-        <v>10911</v>
+        <v>10902</v>
       </c>
       <c r="GZ67" s="0" t="s">
-        <v>10912</v>
+        <v>10903</v>
       </c>
       <c r="HA67" s="0" t="s">
         <v>310</v>
       </c>
       <c r="IC67" s="0" t="s">
-        <v>10913</v>
+        <v>10904</v>
       </c>
       <c r="ID67" s="0" t="s">
-        <v>10914</v>
+        <v>10905</v>
       </c>
       <c r="IE67" s="0" t="s">
-        <v>10915</v>
+        <v>10906</v>
       </c>
       <c r="IF67" s="0" t="s">
-        <v>10916</v>
+        <v>10907</v>
       </c>
       <c r="IG67" s="0" t="s">
         <v>7889</v>
       </c>
       <c r="IH67" s="0" t="s">
-        <v>10917</v>
+        <v>10908</v>
       </c>
       <c r="IJ67" s="0" t="s">
-        <v>10918</v>
+        <v>10909</v>
       </c>
       <c r="IK67" s="0" t="s">
         <v>462</v>
@@ -79470,76 +79450,76 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX68" s="0" t="s">
+        <v>10910</v>
+      </c>
+      <c r="CY68" s="0" t="s">
+        <v>10911</v>
+      </c>
+      <c r="CZ68" s="0" t="s">
+        <v>10912</v>
+      </c>
+      <c r="DA68" s="0" t="s">
+        <v>10913</v>
+      </c>
+      <c r="DB68" s="0" t="s">
+        <v>10914</v>
+      </c>
+      <c r="DC68" s="0" t="s">
+        <v>10915</v>
+      </c>
+      <c r="DD68" s="0" t="s">
+        <v>10916</v>
+      </c>
+      <c r="DE68" s="0" t="s">
+        <v>10917</v>
+      </c>
+      <c r="DF68" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG68" s="0" t="s">
+        <v>10918</v>
+      </c>
+      <c r="DH68" s="0" t="s">
         <v>10919</v>
       </c>
-      <c r="CY68" s="0" t="s">
+      <c r="DI68" s="0" t="s">
         <v>10920</v>
       </c>
-      <c r="CZ68" s="0" t="s">
+      <c r="DJ68" s="0" t="s">
         <v>10921</v>
       </c>
-      <c r="DA68" s="0" t="s">
+      <c r="DK68" s="0" t="s">
         <v>10922</v>
       </c>
-      <c r="DB68" s="0" t="s">
+      <c r="DL68" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM68" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE68" s="0" t="s">
         <v>10923</v>
       </c>
-      <c r="DC68" s="0" t="s">
+      <c r="GF68" s="0" t="s">
         <v>10924</v>
       </c>
-      <c r="DD68" s="0" t="s">
+      <c r="GG68" s="0" t="s">
         <v>10925</v>
       </c>
-      <c r="DE68" s="0" t="s">
+      <c r="GJ68" s="0" t="s">
         <v>10926</v>
       </c>
-      <c r="DF68" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG68" s="0" t="s">
+      <c r="GL68" s="0" t="s">
         <v>10927</v>
       </c>
-      <c r="DH68" s="0" t="s">
+      <c r="GO68" s="0" t="s">
         <v>10928</v>
       </c>
-      <c r="DI68" s="0" t="s">
+      <c r="GP68" s="0" t="s">
         <v>10929</v>
       </c>
-      <c r="DJ68" s="0" t="s">
+      <c r="GQ68" s="0" t="s">
         <v>10930</v>
-      </c>
-      <c r="DK68" s="0" t="s">
-        <v>10931</v>
-      </c>
-      <c r="DL68" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM68" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE68" s="0" t="s">
-        <v>10932</v>
-      </c>
-      <c r="GF68" s="0" t="s">
-        <v>10933</v>
-      </c>
-      <c r="GG68" s="0" t="s">
-        <v>10934</v>
-      </c>
-      <c r="GJ68" s="0" t="s">
-        <v>10935</v>
-      </c>
-      <c r="GL68" s="0" t="s">
-        <v>10936</v>
-      </c>
-      <c r="GO68" s="0" t="s">
-        <v>10937</v>
-      </c>
-      <c r="GP68" s="0" t="s">
-        <v>10938</v>
-      </c>
-      <c r="GQ68" s="0" t="s">
-        <v>10939</v>
       </c>
       <c r="GR68" s="0" t="s">
         <v>310</v>
@@ -79548,126 +79528,126 @@
         <v>370</v>
       </c>
       <c r="GT68" s="0" t="s">
-        <v>10905</v>
+        <v>10896</v>
       </c>
       <c r="GU68" s="0" t="s">
+        <v>10931</v>
+      </c>
+      <c r="GV68" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW68" s="0" t="s">
+        <v>10932</v>
+      </c>
+      <c r="GX68" s="0" t="s">
+        <v>10933</v>
+      </c>
+      <c r="GY68" s="0" t="s">
+        <v>10934</v>
+      </c>
+      <c r="GZ68" s="0" t="s">
+        <v>10935</v>
+      </c>
+      <c r="HA68" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC68" s="0" t="s">
+        <v>10936</v>
+      </c>
+      <c r="ID68" s="0" t="s">
+        <v>10937</v>
+      </c>
+      <c r="IE68" s="0" t="s">
+        <v>10938</v>
+      </c>
+      <c r="IF68" s="0" t="s">
+        <v>10939</v>
+      </c>
+      <c r="IG68" s="0" t="s">
         <v>10940</v>
       </c>
-      <c r="GV68" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW68" s="0" t="s">
+      <c r="IH68" s="0" t="s">
         <v>10941</v>
       </c>
-      <c r="GX68" s="0" t="s">
+      <c r="IJ68" s="0" t="s">
         <v>10942</v>
       </c>
-      <c r="GY68" s="0" t="s">
+      <c r="IK68" s="0" t="s">
         <v>10943</v>
-      </c>
-      <c r="GZ68" s="0" t="s">
-        <v>10944</v>
-      </c>
-      <c r="HA68" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC68" s="0" t="s">
-        <v>10945</v>
-      </c>
-      <c r="ID68" s="0" t="s">
-        <v>10946</v>
-      </c>
-      <c r="IE68" s="0" t="s">
-        <v>10947</v>
-      </c>
-      <c r="IF68" s="0" t="s">
-        <v>10948</v>
-      </c>
-      <c r="IG68" s="0" t="s">
-        <v>10949</v>
-      </c>
-      <c r="IH68" s="0" t="s">
-        <v>10950</v>
-      </c>
-      <c r="IJ68" s="0" t="s">
-        <v>10951</v>
-      </c>
-      <c r="IK68" s="0" t="s">
-        <v>10952</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX69" s="0" t="s">
+        <v>10944</v>
+      </c>
+      <c r="CY69" s="0" t="s">
+        <v>10945</v>
+      </c>
+      <c r="CZ69" s="0" t="s">
+        <v>10946</v>
+      </c>
+      <c r="DA69" s="0" t="s">
+        <v>10947</v>
+      </c>
+      <c r="DB69" s="0" t="s">
+        <v>10948</v>
+      </c>
+      <c r="DC69" s="0" t="s">
+        <v>10949</v>
+      </c>
+      <c r="DD69" s="0" t="s">
+        <v>10950</v>
+      </c>
+      <c r="DE69" s="0" t="s">
+        <v>10951</v>
+      </c>
+      <c r="DF69" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG69" s="0" t="s">
+        <v>10952</v>
+      </c>
+      <c r="DH69" s="0" t="s">
         <v>10953</v>
       </c>
-      <c r="CY69" s="0" t="s">
+      <c r="DI69" s="0" t="s">
         <v>10954</v>
       </c>
-      <c r="CZ69" s="0" t="s">
+      <c r="DJ69" s="0" t="s">
         <v>10955</v>
       </c>
-      <c r="DA69" s="0" t="s">
+      <c r="DK69" s="0" t="s">
         <v>10956</v>
       </c>
-      <c r="DB69" s="0" t="s">
+      <c r="DL69" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM69" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE69" s="0" t="s">
         <v>10957</v>
       </c>
-      <c r="DC69" s="0" t="s">
+      <c r="GF69" s="0" t="s">
         <v>10958</v>
       </c>
-      <c r="DD69" s="0" t="s">
+      <c r="GG69" s="0" t="s">
         <v>10959</v>
       </c>
-      <c r="DE69" s="0" t="s">
+      <c r="GJ69" s="0" t="s">
         <v>10960</v>
       </c>
-      <c r="DF69" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG69" s="0" t="s">
+      <c r="GL69" s="0" t="s">
         <v>10961</v>
       </c>
-      <c r="DH69" s="0" t="s">
+      <c r="GO69" s="0" t="s">
         <v>10962</v>
       </c>
-      <c r="DI69" s="0" t="s">
+      <c r="GP69" s="0" t="s">
         <v>10963</v>
       </c>
-      <c r="DJ69" s="0" t="s">
+      <c r="GQ69" s="0" t="s">
         <v>10964</v>
-      </c>
-      <c r="DK69" s="0" t="s">
-        <v>10965</v>
-      </c>
-      <c r="DL69" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM69" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE69" s="0" t="s">
-        <v>10966</v>
-      </c>
-      <c r="GF69" s="0" t="s">
-        <v>10967</v>
-      </c>
-      <c r="GG69" s="0" t="s">
-        <v>10968</v>
-      </c>
-      <c r="GJ69" s="0" t="s">
-        <v>10969</v>
-      </c>
-      <c r="GL69" s="0" t="s">
-        <v>10970</v>
-      </c>
-      <c r="GO69" s="0" t="s">
-        <v>10971</v>
-      </c>
-      <c r="GP69" s="0" t="s">
-        <v>10972</v>
-      </c>
-      <c r="GQ69" s="0" t="s">
-        <v>10973</v>
       </c>
       <c r="GR69" s="0" t="s">
         <v>310</v>
@@ -79676,126 +79656,126 @@
         <v>370</v>
       </c>
       <c r="GT69" s="0" t="s">
-        <v>10937</v>
+        <v>10928</v>
       </c>
       <c r="GU69" s="0" t="s">
+        <v>10965</v>
+      </c>
+      <c r="GV69" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW69" s="0" t="s">
+        <v>10966</v>
+      </c>
+      <c r="GX69" s="0" t="s">
+        <v>10967</v>
+      </c>
+      <c r="GY69" s="0" t="s">
+        <v>10968</v>
+      </c>
+      <c r="GZ69" s="0" t="s">
+        <v>10969</v>
+      </c>
+      <c r="HA69" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC69" s="0" t="s">
+        <v>10970</v>
+      </c>
+      <c r="ID69" s="0" t="s">
+        <v>10971</v>
+      </c>
+      <c r="IE69" s="0" t="s">
+        <v>10972</v>
+      </c>
+      <c r="IF69" s="0" t="s">
+        <v>10973</v>
+      </c>
+      <c r="IG69" s="0" t="s">
         <v>10974</v>
       </c>
-      <c r="GV69" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW69" s="0" t="s">
+      <c r="IH69" s="0" t="s">
         <v>10975</v>
       </c>
-      <c r="GX69" s="0" t="s">
+      <c r="IJ69" s="0" t="s">
         <v>10976</v>
       </c>
-      <c r="GY69" s="0" t="s">
+      <c r="IK69" s="0" t="s">
         <v>10977</v>
-      </c>
-      <c r="GZ69" s="0" t="s">
-        <v>10978</v>
-      </c>
-      <c r="HA69" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC69" s="0" t="s">
-        <v>10979</v>
-      </c>
-      <c r="ID69" s="0" t="s">
-        <v>10980</v>
-      </c>
-      <c r="IE69" s="0" t="s">
-        <v>10981</v>
-      </c>
-      <c r="IF69" s="0" t="s">
-        <v>10982</v>
-      </c>
-      <c r="IG69" s="0" t="s">
-        <v>10983</v>
-      </c>
-      <c r="IH69" s="0" t="s">
-        <v>10984</v>
-      </c>
-      <c r="IJ69" s="0" t="s">
-        <v>10985</v>
-      </c>
-      <c r="IK69" s="0" t="s">
-        <v>10986</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX70" s="0" t="s">
+        <v>10978</v>
+      </c>
+      <c r="CY70" s="0" t="s">
+        <v>10979</v>
+      </c>
+      <c r="CZ70" s="0" t="s">
+        <v>10980</v>
+      </c>
+      <c r="DA70" s="0" t="s">
+        <v>10981</v>
+      </c>
+      <c r="DB70" s="0" t="s">
+        <v>10982</v>
+      </c>
+      <c r="DC70" s="0" t="s">
+        <v>10983</v>
+      </c>
+      <c r="DD70" s="0" t="s">
+        <v>10984</v>
+      </c>
+      <c r="DE70" s="0" t="s">
+        <v>10985</v>
+      </c>
+      <c r="DF70" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG70" s="0" t="s">
+        <v>10986</v>
+      </c>
+      <c r="DH70" s="0" t="s">
         <v>10987</v>
       </c>
-      <c r="CY70" s="0" t="s">
+      <c r="DI70" s="0" t="s">
         <v>10988</v>
       </c>
-      <c r="CZ70" s="0" t="s">
+      <c r="DJ70" s="0" t="s">
         <v>10989</v>
       </c>
-      <c r="DA70" s="0" t="s">
+      <c r="DK70" s="0" t="s">
         <v>10990</v>
       </c>
-      <c r="DB70" s="0" t="s">
+      <c r="DL70" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM70" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE70" s="0" t="s">
         <v>10991</v>
       </c>
-      <c r="DC70" s="0" t="s">
+      <c r="GF70" s="0" t="s">
         <v>10992</v>
       </c>
-      <c r="DD70" s="0" t="s">
+      <c r="GG70" s="0" t="s">
         <v>10993</v>
       </c>
-      <c r="DE70" s="0" t="s">
+      <c r="GJ70" s="0" t="s">
         <v>10994</v>
       </c>
-      <c r="DF70" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG70" s="0" t="s">
+      <c r="GL70" s="0" t="s">
         <v>10995</v>
       </c>
-      <c r="DH70" s="0" t="s">
+      <c r="GO70" s="0" t="s">
         <v>10996</v>
       </c>
-      <c r="DI70" s="0" t="s">
+      <c r="GP70" s="0" t="s">
         <v>10997</v>
       </c>
-      <c r="DJ70" s="0" t="s">
+      <c r="GQ70" s="0" t="s">
         <v>10998</v>
-      </c>
-      <c r="DK70" s="0" t="s">
-        <v>10999</v>
-      </c>
-      <c r="DL70" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM70" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE70" s="0" t="s">
-        <v>11000</v>
-      </c>
-      <c r="GF70" s="0" t="s">
-        <v>11001</v>
-      </c>
-      <c r="GG70" s="0" t="s">
-        <v>11002</v>
-      </c>
-      <c r="GJ70" s="0" t="s">
-        <v>11003</v>
-      </c>
-      <c r="GL70" s="0" t="s">
-        <v>11004</v>
-      </c>
-      <c r="GO70" s="0" t="s">
-        <v>11005</v>
-      </c>
-      <c r="GP70" s="0" t="s">
-        <v>11006</v>
-      </c>
-      <c r="GQ70" s="0" t="s">
-        <v>11007</v>
       </c>
       <c r="GR70" s="0" t="s">
         <v>310</v>
@@ -79804,126 +79784,126 @@
         <v>370</v>
       </c>
       <c r="GT70" s="0" t="s">
-        <v>10971</v>
+        <v>10962</v>
       </c>
       <c r="GU70" s="0" t="s">
+        <v>10999</v>
+      </c>
+      <c r="GV70" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW70" s="0" t="s">
+        <v>11000</v>
+      </c>
+      <c r="GX70" s="0" t="s">
+        <v>11001</v>
+      </c>
+      <c r="GY70" s="0" t="s">
+        <v>11002</v>
+      </c>
+      <c r="GZ70" s="0" t="s">
+        <v>11003</v>
+      </c>
+      <c r="HA70" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC70" s="0" t="s">
+        <v>11004</v>
+      </c>
+      <c r="ID70" s="0" t="s">
+        <v>11005</v>
+      </c>
+      <c r="IE70" s="0" t="s">
+        <v>11006</v>
+      </c>
+      <c r="IF70" s="0" t="s">
+        <v>11007</v>
+      </c>
+      <c r="IG70" s="0" t="s">
         <v>11008</v>
       </c>
-      <c r="GV70" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW70" s="0" t="s">
+      <c r="IH70" s="0" t="s">
         <v>11009</v>
       </c>
-      <c r="GX70" s="0" t="s">
+      <c r="IJ70" s="0" t="s">
         <v>11010</v>
       </c>
-      <c r="GY70" s="0" t="s">
+      <c r="IK70" s="0" t="s">
         <v>11011</v>
-      </c>
-      <c r="GZ70" s="0" t="s">
-        <v>11012</v>
-      </c>
-      <c r="HA70" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC70" s="0" t="s">
-        <v>11013</v>
-      </c>
-      <c r="ID70" s="0" t="s">
-        <v>11014</v>
-      </c>
-      <c r="IE70" s="0" t="s">
-        <v>11015</v>
-      </c>
-      <c r="IF70" s="0" t="s">
-        <v>11016</v>
-      </c>
-      <c r="IG70" s="0" t="s">
-        <v>11017</v>
-      </c>
-      <c r="IH70" s="0" t="s">
-        <v>11018</v>
-      </c>
-      <c r="IJ70" s="0" t="s">
-        <v>11019</v>
-      </c>
-      <c r="IK70" s="0" t="s">
-        <v>11020</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="CX71" s="0" t="s">
+        <v>11012</v>
+      </c>
+      <c r="CY71" s="0" t="s">
+        <v>11013</v>
+      </c>
+      <c r="CZ71" s="0" t="s">
+        <v>11014</v>
+      </c>
+      <c r="DA71" s="0" t="s">
+        <v>11015</v>
+      </c>
+      <c r="DB71" s="0" t="s">
+        <v>11016</v>
+      </c>
+      <c r="DC71" s="0" t="s">
+        <v>11017</v>
+      </c>
+      <c r="DD71" s="0" t="s">
+        <v>11018</v>
+      </c>
+      <c r="DE71" s="0" t="s">
+        <v>11019</v>
+      </c>
+      <c r="DF71" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DG71" s="0" t="s">
+        <v>11020</v>
+      </c>
+      <c r="DH71" s="0" t="s">
         <v>11021</v>
       </c>
-      <c r="CY71" s="0" t="s">
+      <c r="DI71" s="0" t="s">
         <v>11022</v>
       </c>
-      <c r="CZ71" s="0" t="s">
+      <c r="DJ71" s="0" t="s">
         <v>11023</v>
       </c>
-      <c r="DA71" s="0" t="s">
+      <c r="DK71" s="0" t="s">
         <v>11024</v>
       </c>
-      <c r="DB71" s="0" t="s">
+      <c r="DL71" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="DM71" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GE71" s="0" t="s">
         <v>11025</v>
       </c>
-      <c r="DC71" s="0" t="s">
+      <c r="GF71" s="0" t="s">
         <v>11026</v>
       </c>
-      <c r="DD71" s="0" t="s">
+      <c r="GG71" s="0" t="s">
         <v>11027</v>
       </c>
-      <c r="DE71" s="0" t="s">
+      <c r="GJ71" s="0" t="s">
         <v>11028</v>
       </c>
-      <c r="DF71" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DG71" s="0" t="s">
+      <c r="GL71" s="0" t="s">
         <v>11029</v>
       </c>
-      <c r="DH71" s="0" t="s">
+      <c r="GO71" s="0" t="s">
         <v>11030</v>
       </c>
-      <c r="DI71" s="0" t="s">
+      <c r="GP71" s="0" t="s">
         <v>11031</v>
       </c>
-      <c r="DJ71" s="0" t="s">
+      <c r="GQ71" s="0" t="s">
         <v>11032</v>
-      </c>
-      <c r="DK71" s="0" t="s">
-        <v>11033</v>
-      </c>
-      <c r="DL71" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="DM71" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GE71" s="0" t="s">
-        <v>11034</v>
-      </c>
-      <c r="GF71" s="0" t="s">
-        <v>11035</v>
-      </c>
-      <c r="GG71" s="0" t="s">
-        <v>11036</v>
-      </c>
-      <c r="GJ71" s="0" t="s">
-        <v>11037</v>
-      </c>
-      <c r="GL71" s="0" t="s">
-        <v>11038</v>
-      </c>
-      <c r="GO71" s="0" t="s">
-        <v>11039</v>
-      </c>
-      <c r="GP71" s="0" t="s">
-        <v>11040</v>
-      </c>
-      <c r="GQ71" s="0" t="s">
-        <v>11041</v>
       </c>
       <c r="GR71" s="0" t="s">
         <v>310</v>
@@ -79932,52 +79912,52 @@
         <v>370</v>
       </c>
       <c r="GT71" s="0" t="s">
-        <v>11005</v>
+        <v>10996</v>
       </c>
       <c r="GU71" s="0" t="s">
+        <v>11033</v>
+      </c>
+      <c r="GV71" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="GW71" s="0" t="s">
+        <v>11034</v>
+      </c>
+      <c r="GX71" s="0" t="s">
+        <v>11035</v>
+      </c>
+      <c r="GY71" s="0" t="s">
+        <v>11036</v>
+      </c>
+      <c r="GZ71" s="0" t="s">
+        <v>11037</v>
+      </c>
+      <c r="HA71" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="IC71" s="0" t="s">
+        <v>11038</v>
+      </c>
+      <c r="ID71" s="0" t="s">
+        <v>11039</v>
+      </c>
+      <c r="IE71" s="0" t="s">
+        <v>11040</v>
+      </c>
+      <c r="IF71" s="0" t="s">
+        <v>11041</v>
+      </c>
+      <c r="IG71" s="0" t="s">
         <v>11042</v>
       </c>
-      <c r="GV71" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="GW71" s="0" t="s">
+      <c r="IH71" s="0" t="s">
         <v>11043</v>
       </c>
-      <c r="GX71" s="0" t="s">
+      <c r="IJ71" s="0" t="s">
         <v>11044</v>
       </c>
-      <c r="GY71" s="0" t="s">
+      <c r="IK71" s="0" t="s">
         <v>11045</v>
-      </c>
-      <c r="GZ71" s="0" t="s">
-        <v>11046</v>
-      </c>
-      <c r="HA71" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="IC71" s="0" t="s">
-        <v>11047</v>
-      </c>
-      <c r="ID71" s="0" t="s">
-        <v>11048</v>
-      </c>
-      <c r="IE71" s="0" t="s">
-        <v>11049</v>
-      </c>
-      <c r="IF71" s="0" t="s">
-        <v>11050</v>
-      </c>
-      <c r="IG71" s="0" t="s">
-        <v>11051</v>
-      </c>
-      <c r="IH71" s="0" t="s">
-        <v>11052</v>
-      </c>
-      <c r="IJ71" s="0" t="s">
-        <v>11053</v>
-      </c>
-      <c r="IK71" s="0" t="s">
-        <v>11054</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -79988,25 +79968,25 @@
         <v>370</v>
       </c>
       <c r="GT72" s="0" t="s">
-        <v>11039</v>
+        <v>11030</v>
       </c>
       <c r="GU72" s="0" t="s">
-        <v>11055</v>
+        <v>11046</v>
       </c>
       <c r="GV72" s="0" t="s">
         <v>310</v>
       </c>
       <c r="GW72" s="0" t="s">
-        <v>11056</v>
+        <v>11047</v>
       </c>
       <c r="GX72" s="0" t="s">
-        <v>11057</v>
+        <v>11048</v>
       </c>
       <c r="GY72" s="0" t="s">
-        <v>11058</v>
+        <v>11049</v>
       </c>
       <c r="GZ72" s="0" t="s">
-        <v>11059</v>
+        <v>11050</v>
       </c>
       <c r="HA72" s="0" t="s">
         <v>310</v>

</xml_diff>